<commit_message>
第十次提交： 1.用例层的编写实战 login_test  quit_test 模块 2.自定义unittest.TestCase SeleniumBaseCase模块
</commit_message>
<xml_diff>
--- a/element_info_datas/element_infos.xlsx
+++ b/element_info_datas/element_infos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\学习资料\python脚本框架\PO_chandao_01_03\elemnt_info_datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\学习资料\python脚本框架\PO_chandao_01_03\element_info_datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E45451-3293-4F1D-9F7F-EAC7E1F86A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91C607F-AF7E-456C-85E0-A886CD0C8AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
   <si>
     <t>元素变量名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//span[@class="user-name"]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>companyname_showbox</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -469,6 +461,28 @@
   </si>
   <si>
     <t>//a[@href="/zentao/task-create-1--0.html"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>退出按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quit_button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//a[@href="/zentao/user-logout.html"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userNav</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>用户菜单</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -856,7 +870,7 @@
     <col min="1" max="1" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="2"/>
@@ -964,7 +978,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>29</v>
@@ -973,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4">
         <v>5</v>
@@ -993,7 +1007,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -1047,13 +1061,13 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -1064,222 +1078,242 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="E11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1334,182 +1368,182 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1561,10 +1595,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -1581,7 +1615,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1601,7 +1635,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -1621,7 +1655,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -1641,27 +1675,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>